<commit_message>
Formatting improved but still issues with left alignment of title columns
</commit_message>
<xml_diff>
--- a/Invalid spatial.xlsx
+++ b/Invalid spatial.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$6</definedName>
+  </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -55,10 +58,10 @@
     <t>avg_area_(m^3)</t>
   </si>
   <si>
+    <t>area_standard_derivation_(+-)</t>
+  </si>
+  <si>
     <t>smallest_area_(m^3)</t>
-  </si>
-  <si>
-    <t>area_standard_derivation_(+-)</t>
   </si>
   <si>
     <t>largest_area_(m^3)</t>
@@ -240,8 +243,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -547,305 +553,321 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="6" width="34.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="65.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>13796</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="1">
         <v>1</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="1">
         <v>90879.7119379221</v>
       </c>
-      <c r="N2">
+      <c r="O2" s="1">
         <v>90879.7119379221</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="1">
         <v>90879.7119379221</v>
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>23065</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="1">
         <v>1</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="1">
         <v>18523.98871062506</v>
       </c>
-      <c r="N3">
+      <c r="O3" s="1">
         <v>18523.98871062506</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="1">
         <v>18523.98871062506</v>
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>23029</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="1">
         <v>26</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="1">
         <v>258149.3249945357</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="1">
+        <v>1104172.958274424</v>
+      </c>
+      <c r="O4" s="1">
         <v>0.000565426327247</v>
       </c>
-      <c r="O4">
-        <v>1104172.958274424</v>
-      </c>
-      <c r="P4">
+      <c r="P4" s="1">
         <v>5587929.031988069</v>
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>23030</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="1">
         <v>4</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="1">
         <v>22304.60178799583</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="1">
+        <v>34568.34476877633</v>
+      </c>
+      <c r="O5" s="1">
         <v>201.2495941353518</v>
       </c>
-      <c r="O5">
-        <v>34568.34476877633</v>
-      </c>
-      <c r="P5">
+      <c r="P5" s="1">
         <v>73850.13623405709</v>
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>25345</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="1">
         <v>14</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="1">
         <v>32831.90971301876</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="1">
+        <v>55474.2487778508</v>
+      </c>
+      <c r="O6" s="1">
         <v>502.8386026041594</v>
       </c>
-      <c r="O6">
-        <v>55474.2487778508</v>
-      </c>
-      <c r="P6">
+      <c r="P6" s="1">
         <v>208631.1298951773</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:R6"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid input" error="Please select an action from the dropdown" sqref="Q2:Q6">
       <formula1>"Corrected,Cancelled,No action required"</formula1>

</xml_diff>